<commit_message>
all code for the PiN is correct and in calculate_PiN.py
</commit_message>
<xml_diff>
--- a/output/Dimension_JIAF_Somalia___SOM.xlsx
+++ b/output/Dimension_JIAF_Somalia___SOM.xlsx
@@ -159,67 +159,41 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>